<commit_message>
added dataProviderAndExcelSheet Test case
</commit_message>
<xml_diff>
--- a/selenium/src/main/java/utilities/Book1.xlsx
+++ b/selenium/src/main/java/utilities/Book1.xlsx
@@ -3,14 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohit\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19275" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,31 +24,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>test123</t>
-  </si>
-  <si>
-    <t>john</t>
-  </si>
-  <si>
-    <t>eva</t>
-  </si>
-  <si>
-    <t>123test</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+  <si>
+    <t>tomsmith</t>
+  </si>
+  <si>
+    <t>SuperSecretPassword!</t>
+  </si>
+  <si>
+    <t>rohit</t>
+  </si>
+  <si>
+    <t>TOMSMITH</t>
+  </si>
+  <si>
+    <t>SuperPassword!</t>
+  </si>
+  <si>
+    <t>testInputPassword</t>
+  </si>
+  <si>
+    <t>testInputUsername</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,16 +65,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -69,14 +94,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -355,43 +398,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>